<commit_message>
* BookType constant name change. (2003 -> XLS, 2007 -> XLSX) * make spring bean name be different from JavaBean name * use separate Excel files for spring bean and JavaBean examples
</commit_message>
<xml_diff>
--- a/3/zssessentials/src/main/webapp/WEB-INF/books/bean.xlsx
+++ b/3/zssessentials/src/main/webapp/WEB-INF/books/bean.xlsx
@@ -300,74 +300,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -379,7 +311,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -659,7 +591,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -702,7 +634,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="23" t="e">
-        <f>assetsBean.liquidAssets</f>
+        <f>myBean.liquidAssets</f>
         <v>#NAME?</v>
       </c>
       <c r="C3" s="10"/>
@@ -717,7 +649,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="23" t="e">
-        <f>assetsBean.fundInvestment</f>
+        <f>myBean.fundInvestment</f>
         <v>#NAME?</v>
       </c>
       <c r="C4" s="10"/>
@@ -732,7 +664,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="23" t="e">
-        <f>assetsBean.fixedAssets</f>
+        <f>myBean.fixedAssets</f>
         <v>#NAME?</v>
       </c>
       <c r="C5" s="10"/>
@@ -747,7 +679,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="23" t="e">
-        <f>assetsBean.intangibleAsset</f>
+        <f>myBean.intangibleAsset</f>
         <v>#NAME?</v>
       </c>
       <c r="C6" s="10"/>
@@ -761,7 +693,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="23" t="e">
-        <f>assetsBean.otherAssets</f>
+        <f>myBean.otherAssets</f>
         <v>#NAME?</v>
       </c>
       <c r="C7" s="10"/>

</xml_diff>